<commit_message>
Fixed button positioning bug
</commit_message>
<xml_diff>
--- a/data/first_order_ode.xlsx
+++ b/data/first_order_ode.xlsx
@@ -375,234 +375,234 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>0.103448275862069</v>
+        <v>0.06896551724137931</v>
       </c>
       <c r="B3">
-        <v>1.092746730083234</v>
+        <v>1.068965517241379</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>0.2068965517241379</v>
+        <v>0.1379310344827586</v>
       </c>
       <c r="B4">
-        <v>1.184386403706589</v>
+        <v>1.14268727705113</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>0.3103448275862069</v>
+        <v>0.2068965517241379</v>
       </c>
       <c r="B5">
-        <v>1.274804497788008</v>
+        <v>1.221493296158104</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>0.4137931034482759</v>
+        <v>0.2758620689655172</v>
       </c>
       <c r="B6">
-        <v>1.363874642030049</v>
+        <v>1.305734213134525</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>0.5172413793103449</v>
+        <v>0.3448275862068966</v>
       </c>
       <c r="B7">
-        <v>1.451457393345881</v>
+        <v>1.395784848523113</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>0.6206896551724138</v>
+        <v>0.4137931034482759</v>
       </c>
       <c r="B8">
-        <v>1.537398883501756</v>
+        <v>1.49204587255919</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>0.7241379310344828</v>
+        <v>0.4827586206896551</v>
       </c>
       <c r="B9">
-        <v>1.62152932686044</v>
+        <v>1.594945587908099</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>0.8275862068965517</v>
+        <v>0.5517241379310345</v>
       </c>
       <c r="B10">
-        <v>1.703661373753256</v>
+        <v>1.704941835350037</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>0.9310344827586207</v>
+        <v>0.6206896551724138</v>
       </c>
       <c r="B11">
-        <v>1.783588293511322</v>
+        <v>1.822524030891419</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>1.03448275862069</v>
+        <v>0.6896551724137931</v>
       </c>
       <c r="B12">
-        <v>1.86108196953449</v>
+        <v>1.948215343366689</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>1.137931034482759</v>
+        <v>0.7586206896551724</v>
       </c>
       <c r="B13">
-        <v>1.935890686953635</v>
+        <v>2.082575022219564</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>1.241379310344828</v>
+        <v>0.8275862068965517</v>
       </c>
       <c r="B14">
-        <v>2.007736691430408</v>
+        <v>2.226200885820913</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>1.344827586206897</v>
+        <v>0.896551724137931</v>
       </c>
       <c r="B15">
-        <v>2.076313495419047</v>
+        <v>2.379731981394769</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>1.448275862068966</v>
+        <v>0.9655172413793103</v>
       </c>
       <c r="B16">
-        <v>2.141282905765608</v>
+        <v>2.543851428387512</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>1.551724137931034</v>
+        <v>1.03448275862069</v>
       </c>
       <c r="B17">
-        <v>2.20227174381746</v>
+        <v>2.719289457931478</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>1.655172413793103</v>
+        <v>1.103448275862069</v>
       </c>
       <c r="B18">
-        <v>2.258868226233773</v>
+        <v>2.906826661926753</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>1.758620689655172</v>
+        <v>1.172413793103448</v>
       </c>
       <c r="B19">
-        <v>2.310617971397076</v>
+        <v>3.107297466197563</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>1.862068965517241</v>
+        <v>1.241379310344828</v>
       </c>
       <c r="B20">
-        <v>2.35701959269499</v>
+        <v>3.321593843176705</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>1.96551724137931</v>
+        <v>1.310344827586207</v>
       </c>
       <c r="B21">
-        <v>2.397519835934543</v>
+        <v>3.550669280637168</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>2.068965517241379</v>
+        <v>1.379310344827586</v>
       </c>
       <c r="B22">
-        <v>2.431508213730388</v>
+        <v>3.795543024129386</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>2.172413793103448</v>
+        <v>1.448275862068966</v>
       </c>
       <c r="B23">
-        <v>2.458311084829726</v>
+        <v>4.057304612000379</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>2.275862068965517</v>
+        <v>1.517241379310345</v>
       </c>
       <c r="B24">
-        <v>2.47718512095361</v>
+        <v>4.337118723172819</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
-        <v>2.379310344827586</v>
+        <v>1.586206896551724</v>
       </c>
       <c r="B25">
-        <v>2.487310097794234</v>
+        <v>4.636230359253703</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>2.482758620689655</v>
+        <v>1.655172413793103</v>
       </c>
       <c r="B26">
-        <v>2.487780940253328</v>
+        <v>4.95597038402982</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>2.586206896551724</v>
+        <v>1.724137931034483</v>
       </c>
       <c r="B27">
-        <v>2.477598944774184</v>
+        <v>5.297761444997394</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>2.689655172413793</v>
+        <v>1.793103448275862</v>
       </c>
       <c r="B28">
-        <v>2.455662093639052</v>
+        <v>5.663124303273077</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>2.793103448275862</v>
+        <v>1.862068965517241</v>
       </c>
       <c r="B29">
-        <v>2.420754367297313</v>
+        <v>6.053684600050531</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>2.896551724137931</v>
+        <v>1.931034482758621</v>
       </c>
       <c r="B30">
-        <v>2.371533951072422</v>
+        <v>6.471180089709188</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B31">
-        <v>2.306520221873017</v>
+        <v>6.917468371758098</v>
       </c>
     </row>
   </sheetData>

</xml_diff>